<commit_message>
changes to computational and new results for different sizes
</commit_message>
<xml_diff>
--- a/size 68.xlsx
+++ b/size 68.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Documents\studia\C\draw, paint, repeat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Documents\studia\C\Draw-paint-repeat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91AE6BC-3460-4651-8CB3-D2CB11B800FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6107296E-3969-4FDF-BAEC-27112D0CE397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC8F2B7-844E-4FA4-A935-03493D274A6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6CC8F2B7-844E-4FA4-A935-03493D274A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t># of tries</t>
   </si>
@@ -46,6 +47,48 @@
   </si>
   <si>
     <t>% that this or any previous was last</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>xw</t>
+  </si>
+  <si>
+    <t>yw</t>
+  </si>
+  <si>
+    <t># of balls</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>f(x)</t>
+  </si>
+  <si>
+    <t>f(x) = 9,5</t>
+  </si>
+  <si>
+    <t>x=</t>
+  </si>
+  <si>
+    <t>f(x) = 10,5</t>
   </si>
 </sst>
 </file>
@@ -82,9 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -180,14 +226,16 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -207,12 +255,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$69</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -254,386 +347,62 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$69</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="68"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4918000000000001E-2</c:v>
+                  <c:v>1.1695000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8903000000000002E-2</c:v>
+                  <c:v>2.2950999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2236999999999997E-2</c:v>
+                  <c:v>3.3838E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3952E-2</c:v>
+                  <c:v>4.3284000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2984999999999999E-2</c:v>
+                  <c:v>5.176E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.9966E-2</c:v>
+                  <c:v>5.8691E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5507000000000005E-2</c:v>
+                  <c:v>6.3122999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.6486999999999999E-2</c:v>
+                  <c:v>6.6743999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.6309000000000002E-2</c:v>
+                  <c:v>6.7571999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.3549000000000003E-2</c:v>
+                  <c:v>6.7322000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.8723000000000006E-2</c:v>
+                  <c:v>6.5420000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3020999999999994E-2</c:v>
+                  <c:v>6.2615000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5745999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.8917000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.1531999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.4803000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.8156E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.2342000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.7246000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.3096E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.7890000000000008E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.1209999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.9500000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.4589999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.2620000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.5679999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.9299999999999996E-4</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6.0300000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.8900000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.04E-4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.2400000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.8999999999999997E-5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.1E-5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.1999999999999999E-5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6.0000000000000002E-6</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.9999999999999999E-6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.9999999999999999E-6</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.9999999999999995E-7</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
+                  <c:v>5.8321999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C2B0-4210-AE23-281B123C22AA}"/>
@@ -655,6 +424,8 @@
         <c:axId val="892421039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1154,205 +925,205 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4918000000000001E-2</c:v>
+                  <c:v>1.1695000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3820999999999999E-2</c:v>
+                  <c:v>3.4645999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6057999999999996E-2</c:v>
+                  <c:v>6.8483999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14001</c:v>
+                  <c:v>0.11176799999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20299499999999998</c:v>
+                  <c:v>0.16352800000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27296100000000001</c:v>
+                  <c:v>0.222219</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.348468</c:v>
+                  <c:v>0.28534199999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.42495499999999997</c:v>
+                  <c:v>0.35208600000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50126399999999993</c:v>
+                  <c:v>0.41965799999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.57481299999999991</c:v>
+                  <c:v>0.48697999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.64353599999999989</c:v>
+                  <c:v>0.5524</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.70655699999999988</c:v>
+                  <c:v>0.61501499999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.76230299999999984</c:v>
+                  <c:v>0.67333699999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81121999999999983</c:v>
+                  <c:v>0.72660099999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.85275199999999984</c:v>
+                  <c:v>0.77426699999999993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88755499999999987</c:v>
+                  <c:v>0.81647999999999987</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.91571099999999983</c:v>
+                  <c:v>0.85258099999999992</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9380529999999998</c:v>
+                  <c:v>0.88340999999999992</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.95529899999999979</c:v>
+                  <c:v>0.90904199999999991</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.96839499999999978</c:v>
+                  <c:v>0.93024799999999985</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.97818399999999983</c:v>
+                  <c:v>0.94722099999999987</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.98530499999999988</c:v>
+                  <c:v>0.96060999999999985</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.99025499999999989</c:v>
+                  <c:v>0.97096399999999983</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99371399999999988</c:v>
+                  <c:v>0.97910299999999983</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99597599999999986</c:v>
+                  <c:v>0.98512199999999983</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99754399999999988</c:v>
+                  <c:v>0.98962899999999987</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.9985369999999999</c:v>
+                  <c:v>0.99286999999999992</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99913999999999992</c:v>
+                  <c:v>0.99514799999999992</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99952899999999989</c:v>
+                  <c:v>0.99677399999999994</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99973299999999987</c:v>
+                  <c:v>0.99790799999999991</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.99985699999999988</c:v>
+                  <c:v>0.99866799999999989</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.99992599999999987</c:v>
+                  <c:v>0.99914799999999993</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.99996699999999983</c:v>
+                  <c:v>0.99947799999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99998899999999979</c:v>
+                  <c:v>0.99969200000000003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.99999499999999975</c:v>
+                  <c:v>0.999834</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.99999699999999969</c:v>
+                  <c:v>0.99990100000000004</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.99999899999999964</c:v>
+                  <c:v>0.999942</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.99999899999999964</c:v>
+                  <c:v>0.99996600000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.99999899999999964</c:v>
+                  <c:v>0.99998200000000004</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>0.99998900000000002</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>0.99999499999999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>0.99999699999999991</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>0.99999799999999994</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>0.99999899999999997</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.99999999999999967</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,6 +1324,387 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C61-4902-AA83-8F6B8ECF6106}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1477750496"/>
+        <c:axId val="1464888784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1477750496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="92"/>
+          <c:min val="58"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1464888784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1464888784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1477750496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1633,6 +1785,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2150,6 +2342,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2734,6 +3442,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D1674A-8EFF-4DE9-8908-F6166348EE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3039,10 +3788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8E7F59-D6D8-4ABF-84C8-6C12B89D4CFD}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,6 +3800,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f>B2/$B$70</f>
+        <f>B2/$B$100</f>
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -3088,15 +3838,15 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14918</v>
+        <v>11695</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C66" si="0">B3/$B$70</f>
-        <v>1.4918000000000001E-2</v>
+        <f>B3/$B$100</f>
+        <v>1.1695000000000001E-2</v>
       </c>
       <c r="D3" s="1">
         <f>SUM($C$2:C3)</f>
-        <v>1.4918000000000001E-2</v>
+        <v>1.1695000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3104,15 +3854,15 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28903</v>
+        <v>22951</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8903000000000002E-2</v>
+        <f>B4/$B$100</f>
+        <v>2.2950999999999999E-2</v>
       </c>
       <c r="D4" s="1">
         <f>SUM($C$2:C4)</f>
-        <v>4.3820999999999999E-2</v>
+        <v>3.4645999999999996E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3120,15 +3870,15 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>42237</v>
+        <v>33838</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>4.2236999999999997E-2</v>
+        <f>B5/$B$100</f>
+        <v>3.3838E-2</v>
       </c>
       <c r="D5" s="1">
         <f>SUM($C$2:C5)</f>
-        <v>8.6057999999999996E-2</v>
+        <v>6.8483999999999989E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3136,15 +3886,15 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>53952</v>
+        <v>43284</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3952E-2</v>
+        <f>B6/$B$100</f>
+        <v>4.3284000000000003E-2</v>
       </c>
       <c r="D6" s="1">
         <f>SUM($C$2:C6)</f>
-        <v>0.14001</v>
+        <v>0.11176799999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,15 +3902,15 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>62985</v>
+        <v>51760</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>6.2984999999999999E-2</v>
+        <f>B7/$B$100</f>
+        <v>5.176E-2</v>
       </c>
       <c r="D7" s="1">
         <f>SUM($C$2:C7)</f>
-        <v>0.20299499999999998</v>
+        <v>0.16352800000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3168,15 +3918,15 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>69966</v>
+        <v>58691</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>6.9966E-2</v>
+        <f>B8/$B$100</f>
+        <v>5.8691E-2</v>
       </c>
       <c r="D8" s="1">
         <f>SUM($C$2:C8)</f>
-        <v>0.27296100000000001</v>
+        <v>0.222219</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3184,15 +3934,15 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>75507</v>
+        <v>63123</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>7.5507000000000005E-2</v>
+        <f>B9/$B$100</f>
+        <v>6.3122999999999999E-2</v>
       </c>
       <c r="D9" s="1">
         <f>SUM($C$2:C9)</f>
-        <v>0.348468</v>
+        <v>0.28534199999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3200,15 +3950,15 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>76487</v>
+        <v>66744</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>7.6486999999999999E-2</v>
+        <f>B10/$B$100</f>
+        <v>6.6743999999999998E-2</v>
       </c>
       <c r="D10" s="1">
         <f>SUM($C$2:C10)</f>
-        <v>0.42495499999999997</v>
+        <v>0.35208600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3216,15 +3966,15 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>76309</v>
+        <v>67572</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>7.6309000000000002E-2</v>
+        <f>B11/$B$100</f>
+        <v>6.7571999999999993E-2</v>
       </c>
       <c r="D11" s="1">
         <f>SUM($C$2:C11)</f>
-        <v>0.50126399999999993</v>
+        <v>0.41965799999999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3232,15 +3982,15 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>73549</v>
+        <v>67322</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>7.3549000000000003E-2</v>
+        <f>B12/$B$100</f>
+        <v>6.7322000000000007E-2</v>
       </c>
       <c r="D12" s="1">
         <f>SUM($C$2:C12)</f>
-        <v>0.57481299999999991</v>
+        <v>0.48697999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3248,15 +3998,15 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>68723</v>
+        <v>65420</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>6.8723000000000006E-2</v>
+        <f>B13/$B$100</f>
+        <v>6.5420000000000006E-2</v>
       </c>
       <c r="D13" s="1">
         <f>SUM($C$2:C13)</f>
-        <v>0.64353599999999989</v>
+        <v>0.5524</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,15 +4014,15 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>63021</v>
+        <v>62615</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>6.3020999999999994E-2</v>
+        <f>B14/$B$100</f>
+        <v>6.2615000000000004E-2</v>
       </c>
       <c r="D14" s="1">
         <f>SUM($C$2:C14)</f>
-        <v>0.70655699999999988</v>
+        <v>0.61501499999999998</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,15 +4030,15 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>55746</v>
+        <v>58322</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
-        <v>5.5745999999999997E-2</v>
+        <f>B15/$B$100</f>
+        <v>5.8321999999999999E-2</v>
       </c>
       <c r="D15" s="1">
         <f>SUM($C$2:C15)</f>
-        <v>0.76230299999999984</v>
+        <v>0.67333699999999996</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3296,271 +4046,299 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>48917</v>
+        <v>53264</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>4.8917000000000002E-2</v>
+        <f>B16/$B$100</f>
+        <v>5.3263999999999999E-2</v>
       </c>
       <c r="D16" s="1">
         <f>SUM($C$2:C16)</f>
-        <v>0.81121999999999983</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.72660099999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>41532</v>
+        <v>47666</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>4.1531999999999999E-2</v>
+        <f>B17/$B$100</f>
+        <v>4.7666E-2</v>
       </c>
       <c r="D17" s="1">
         <f>SUM($C$2:C17)</f>
-        <v>0.85275199999999984</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.77426699999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>34803</v>
+        <v>42213</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4803000000000001E-2</v>
+        <f>B18/$B$100</f>
+        <v>4.2213000000000001E-2</v>
       </c>
       <c r="D18" s="1">
         <f>SUM($C$2:C18)</f>
-        <v>0.88755499999999987</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.81647999999999987</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>28156</v>
+        <v>36101</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8156E-2</v>
+        <f>B19/$B$100</f>
+        <v>3.6101000000000001E-2</v>
       </c>
       <c r="D19" s="1">
         <f>SUM($C$2:C19)</f>
-        <v>0.91571099999999983</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.85258099999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>22342</v>
+        <v>30829</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2342000000000001E-2</v>
+        <f>B20/$B$100</f>
+        <v>3.0828999999999999E-2</v>
       </c>
       <c r="D20" s="1">
         <f>SUM($C$2:C20)</f>
-        <v>0.9380529999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.88340999999999992</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>-7.5900000000000002E-4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <f>-J21/(2*J20)</f>
+        <v>10.552042160737813</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>17246</v>
+        <v>25632</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7246000000000001E-2</v>
+        <f>B21/$B$100</f>
+        <v>2.5631999999999999E-2</v>
       </c>
       <c r="D21" s="1">
         <f>SUM($C$2:C21)</f>
-        <v>0.95529899999999979</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.90904199999999991</v>
+      </c>
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>1.6018000000000001E-2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>13096</v>
+        <v>21206</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
-        <v>1.3096E-2</v>
+        <f>B22/$B$100</f>
+        <v>2.1205999999999999E-2</v>
       </c>
       <c r="D22" s="1">
         <f>SUM($C$2:C22)</f>
-        <v>0.96839499999999978</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.93024799999999985</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>-1.6E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>9789</v>
+        <v>16973</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>9.7890000000000008E-3</v>
+        <f>B23/$B$100</f>
+        <v>1.6972999999999999E-2</v>
       </c>
       <c r="D23" s="1">
         <f>SUM($C$2:C23)</f>
-        <v>0.97818399999999983</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.94722099999999987</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>7121</v>
+        <v>13389</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>7.1209999999999997E-3</v>
+        <f>B24/$B$100</f>
+        <v>1.3389E-2</v>
       </c>
       <c r="D24" s="1">
         <f>SUM($C$2:C24)</f>
-        <v>0.98530499999999988</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.96060999999999985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>4950</v>
+        <v>10354</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9500000000000004E-3</v>
+        <f>B25/$B$100</f>
+        <v>1.0354E-2</v>
       </c>
       <c r="D25" s="1">
         <f>SUM($C$2:C25)</f>
-        <v>0.99025499999999989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.97096399999999983</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>3459</v>
+        <v>8139</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4589999999999998E-3</v>
+        <f>B26/$B$100</f>
+        <v>8.1390000000000004E-3</v>
       </c>
       <c r="D26" s="1">
         <f>SUM($C$2:C26)</f>
-        <v>0.99371399999999988</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.97910299999999983</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2262</v>
+        <v>6019</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2620000000000001E-3</v>
+        <f>B27/$B$100</f>
+        <v>6.019E-3</v>
       </c>
       <c r="D27" s="1">
         <f>SUM($C$2:C27)</f>
-        <v>0.99597599999999986</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.98512199999999983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1568</v>
+        <v>4507</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5679999999999999E-3</v>
+        <f>B28/$B$100</f>
+        <v>4.5069999999999997E-3</v>
       </c>
       <c r="D28" s="1">
         <f>SUM($C$2:C28)</f>
-        <v>0.99754399999999988</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.98962899999999987</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>993</v>
+        <v>3241</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="0"/>
-        <v>9.9299999999999996E-4</v>
+        <f>B29/$B$100</f>
+        <v>3.241E-3</v>
       </c>
       <c r="D29" s="1">
         <f>SUM($C$2:C29)</f>
-        <v>0.9985369999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.99286999999999992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>603</v>
+        <v>2278</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="0"/>
-        <v>6.0300000000000002E-4</v>
+        <f>B30/$B$100</f>
+        <v>2.2780000000000001E-3</v>
       </c>
       <c r="D30" s="1">
         <f>SUM($C$2:C30)</f>
-        <v>0.99913999999999992</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.99514799999999992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>389</v>
+        <v>1626</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="0"/>
-        <v>3.8900000000000002E-4</v>
+        <f>B31/$B$100</f>
+        <v>1.6260000000000001E-3</v>
       </c>
       <c r="D31" s="1">
         <f>SUM($C$2:C31)</f>
-        <v>0.99952899999999989</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.99677399999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>204</v>
+        <v>1134</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="0"/>
-        <v>2.04E-4</v>
+        <f>B32/$B$100</f>
+        <v>1.134E-3</v>
       </c>
       <c r="D32" s="1">
         <f>SUM($C$2:C32)</f>
-        <v>0.99973299999999987</v>
+        <v>0.99790799999999991</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,15 +4346,15 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>124</v>
+        <v>760</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2400000000000001E-4</v>
+        <f>B33/$B$100</f>
+        <v>7.6000000000000004E-4</v>
       </c>
       <c r="D33" s="1">
         <f>SUM($C$2:C33)</f>
-        <v>0.99985699999999988</v>
+        <v>0.99866799999999989</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,15 +4362,15 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>69</v>
+        <v>480</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="0"/>
-        <v>6.8999999999999997E-5</v>
+        <f>B34/$B$100</f>
+        <v>4.8000000000000001E-4</v>
       </c>
       <c r="D34" s="1">
         <f>SUM($C$2:C34)</f>
-        <v>0.99992599999999987</v>
+        <v>0.99914799999999993</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,15 +4378,15 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>41</v>
+        <v>330</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="0"/>
-        <v>4.1E-5</v>
+        <f>B35/$B$100</f>
+        <v>3.3E-4</v>
       </c>
       <c r="D35" s="1">
         <f>SUM($C$2:C35)</f>
-        <v>0.99996699999999983</v>
+        <v>0.99947799999999998</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,15 +4394,15 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>214</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-5</v>
+        <f>B36/$B$100</f>
+        <v>2.14E-4</v>
       </c>
       <c r="D36" s="1">
         <f>SUM($C$2:C36)</f>
-        <v>0.99998899999999979</v>
+        <v>0.99969200000000003</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,15 +4410,15 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="0"/>
-        <v>6.0000000000000002E-6</v>
+        <f>B37/$B$100</f>
+        <v>1.4200000000000001E-4</v>
       </c>
       <c r="D37" s="1">
         <f>SUM($C$2:C37)</f>
-        <v>0.99999499999999975</v>
+        <v>0.999834</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,15 +4426,15 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999999E-6</v>
+        <f>B38/$B$100</f>
+        <v>6.7000000000000002E-5</v>
       </c>
       <c r="D38" s="1">
         <f>SUM($C$2:C38)</f>
-        <v>0.99999699999999969</v>
+        <v>0.99990100000000004</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,15 +4442,15 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999999E-6</v>
+        <f>B39/$B$100</f>
+        <v>4.1E-5</v>
       </c>
       <c r="D39" s="1">
         <f>SUM($C$2:C39)</f>
-        <v>0.99999899999999964</v>
+        <v>0.999942</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,15 +4458,15 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B40/$B$100</f>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="D40" s="1">
         <f>SUM($C$2:C40)</f>
-        <v>0.99999899999999964</v>
+        <v>0.99996600000000002</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3696,15 +4474,15 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B41/$B$100</f>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="D41" s="1">
         <f>SUM($C$2:C41)</f>
-        <v>0.99999899999999964</v>
+        <v>0.99998200000000004</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,15 +4490,15 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
+        <f>B42/$B$100</f>
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="D42" s="1">
         <f>SUM($C$2:C42)</f>
-        <v>0.99999999999999967</v>
+        <v>0.99998900000000002</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3728,15 +4506,15 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B43/$B$100</f>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="D43" s="1">
         <f>SUM($C$2:C43)</f>
-        <v>0.99999999999999967</v>
+        <v>0.99999499999999997</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,15 +4522,15 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B44/$B$100</f>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="D44" s="1">
         <f>SUM($C$2:C44)</f>
-        <v>0.99999999999999967</v>
+        <v>0.99999699999999991</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3760,15 +4538,15 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B45/$B$100</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D45" s="1">
         <f>SUM($C$2:C45)</f>
-        <v>0.99999999999999967</v>
+        <v>0.99999799999999994</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,15 +4554,15 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B46/$B$100</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D46" s="1">
         <f>SUM($C$2:C46)</f>
-        <v>0.99999999999999967</v>
+        <v>0.99999899999999997</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3792,15 +4570,15 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B47/$B$100</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D47" s="1">
         <f>SUM($C$2:C47)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,12 +4589,12 @@
         <v>0</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="0"/>
+        <f>B48/$B$100</f>
         <v>0</v>
       </c>
       <c r="D48" s="1">
         <f>SUM($C$2:C48)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,12 +4605,12 @@
         <v>0</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="0"/>
+        <f>B49/$B$100</f>
         <v>0</v>
       </c>
       <c r="D49" s="1">
         <f>SUM($C$2:C49)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3843,12 +4621,12 @@
         <v>0</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="0"/>
+        <f>B50/$B$100</f>
         <v>0</v>
       </c>
       <c r="D50" s="1">
         <f>SUM($C$2:C50)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3859,12 +4637,12 @@
         <v>0</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="0"/>
+        <f>B51/$B$100</f>
         <v>0</v>
       </c>
       <c r="D51" s="1">
         <f>SUM($C$2:C51)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,12 +4653,12 @@
         <v>0</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="0"/>
+        <f>B52/$B$100</f>
         <v>0</v>
       </c>
       <c r="D52" s="1">
         <f>SUM($C$2:C52)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3891,12 +4669,12 @@
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="0"/>
+        <f>B53/$B$100</f>
         <v>0</v>
       </c>
       <c r="D53" s="1">
         <f>SUM($C$2:C53)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3907,12 +4685,12 @@
         <v>0</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="0"/>
+        <f>B54/$B$100</f>
         <v>0</v>
       </c>
       <c r="D54" s="1">
         <f>SUM($C$2:C54)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3923,12 +4701,12 @@
         <v>0</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="0"/>
+        <f>B55/$B$100</f>
         <v>0</v>
       </c>
       <c r="D55" s="1">
         <f>SUM($C$2:C55)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3939,12 +4717,12 @@
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="0"/>
+        <f>B56/$B$100</f>
         <v>0</v>
       </c>
       <c r="D56" s="1">
         <f>SUM($C$2:C56)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,12 +4733,12 @@
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" si="0"/>
+        <f>B57/$B$100</f>
         <v>0</v>
       </c>
       <c r="D57" s="1">
         <f>SUM($C$2:C57)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,12 +4749,12 @@
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="0"/>
+        <f>B58/$B$100</f>
         <v>0</v>
       </c>
       <c r="D58" s="1">
         <f>SUM($C$2:C58)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3987,12 +4765,12 @@
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="0"/>
+        <f>B59/$B$100</f>
         <v>0</v>
       </c>
       <c r="D59" s="1">
         <f>SUM($C$2:C59)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4003,12 +4781,12 @@
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" si="0"/>
+        <f>B60/$B$100</f>
         <v>0</v>
       </c>
       <c r="D60" s="1">
         <f>SUM($C$2:C60)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4019,12 +4797,12 @@
         <v>0</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" si="0"/>
+        <f>B61/$B$100</f>
         <v>0</v>
       </c>
       <c r="D61" s="1">
         <f>SUM($C$2:C61)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,12 +4813,12 @@
         <v>0</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" si="0"/>
+        <f>B62/$B$100</f>
         <v>0</v>
       </c>
       <c r="D62" s="1">
         <f>SUM($C$2:C62)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4051,12 +4829,12 @@
         <v>0</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" si="0"/>
+        <f>B63/$B$100</f>
         <v>0</v>
       </c>
       <c r="D63" s="1">
         <f>SUM($C$2:C63)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4067,12 +4845,12 @@
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" si="0"/>
+        <f>B64/$B$100</f>
         <v>0</v>
       </c>
       <c r="D64" s="1">
         <f>SUM($C$2:C64)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,12 +4861,12 @@
         <v>0</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" si="0"/>
+        <f>B65/$B$100</f>
         <v>0</v>
       </c>
       <c r="D65" s="1">
         <f>SUM($C$2:C65)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4099,12 +4877,12 @@
         <v>0</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" si="0"/>
+        <f>B66/$B$100</f>
         <v>0</v>
       </c>
       <c r="D66" s="1">
         <f>SUM($C$2:C66)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,12 +4893,12 @@
         <v>0</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" ref="C67:C69" si="1">B67/$B$70</f>
+        <f>B67/$B$100</f>
         <v>0</v>
       </c>
       <c r="D67" s="1">
         <f>SUM($C$2:C67)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4131,12 +4909,12 @@
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" si="1"/>
+        <f>B68/$B$100</f>
         <v>0</v>
       </c>
       <c r="D68" s="1">
         <f>SUM($C$2:C68)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,17 +4925,130 @@
         <v>0</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" si="1"/>
+        <f>B69/$B$100</f>
         <v>0</v>
       </c>
       <c r="D69" s="1">
         <f>SUM($C$2:C69)</f>
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
       <c r="B70">
-        <f>SUM(B2:B69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <f>SUM(B2:B70)</f>
         <v>1000000</v>
       </c>
     </row>
@@ -4166,4 +5057,142 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EA1655-7A5E-440C-8DD1-9D0D88809235}">
+  <dimension ref="B3:AB14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>10.85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>9.39</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9" s="2">
+        <v>5.6899999999999999E-2</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" s="2">
+        <v>5.6609999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>10.31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>86</v>
+      </c>
+      <c r="C11">
+        <v>10.55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="Y13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB13">
+        <f>(9.5-5.661)/U9</f>
+        <v>67.469244288224971</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="Y14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB14">
+        <f>(10.5-X9)/U9</f>
+        <v>85.043936731107209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>